<commit_message>
Added versions; added short labels using skosxl
</commit_message>
<xml_diff>
--- a/ilearn/generate-onderwijsstructuur/input/onderwijsstructuur.xlsx
+++ b/ilearn/generate-onderwijsstructuur/input/onderwijsstructuur.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="191">
   <si>
     <t>mapping</t>
   </si>
@@ -516,6 +516,87 @@
   </si>
   <si>
     <t>buitengewoon lager onderwijs</t>
+  </si>
+  <si>
+    <t>kortLabel</t>
+  </si>
+  <si>
+    <t>1e graad</t>
+  </si>
+  <si>
+    <t>1e leerjaar</t>
+  </si>
+  <si>
+    <t>2e leerjaar</t>
+  </si>
+  <si>
+    <t>2e graad</t>
+  </si>
+  <si>
+    <t>3e leerjaar</t>
+  </si>
+  <si>
+    <t>4e leerjaar</t>
+  </si>
+  <si>
+    <t>3e graad</t>
+  </si>
+  <si>
+    <t>5e leerjaar</t>
+  </si>
+  <si>
+    <t>6e leerjaar</t>
+  </si>
+  <si>
+    <t>7e leerjaar</t>
+  </si>
+  <si>
+    <t>a-stroom</t>
+  </si>
+  <si>
+    <t>b-stroom</t>
+  </si>
+  <si>
+    <t>finaliteit doorstroom</t>
+  </si>
+  <si>
+    <t>aso</t>
+  </si>
+  <si>
+    <t>tso</t>
+  </si>
+  <si>
+    <t>kso</t>
+  </si>
+  <si>
+    <t>dubbele finaliteit</t>
+  </si>
+  <si>
+    <t>finaliteit arbeidsmarkt</t>
+  </si>
+  <si>
+    <t>bso</t>
+  </si>
+  <si>
+    <t>3e graad 3e leerjaar</t>
+  </si>
+  <si>
+    <t>versie</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>buitengewoon secundair opleidingsvorm 1</t>
+  </si>
+  <si>
+    <t>buitengewoon secundair opleidingsvorm 2</t>
+  </si>
+  <si>
+    <t>buitengewoon secundair opleidingsvorm 3</t>
+  </si>
+  <si>
+    <t>buitengewoon secundair opleidingsvorm 4</t>
   </si>
 </sst>
 </file>
@@ -875,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" topLeftCell="H40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -892,11 +973,11 @@
     <col min="7" max="7" width="27.85546875" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" customWidth="1"/>
     <col min="9" max="9" width="43.28515625" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="47" style="2" customWidth="1"/>
+    <col min="10" max="11" width="50" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -930,8 +1011,14 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -942,8 +1029,11 @@
         <f t="shared" ref="K2:K12" si="0">J2</f>
         <v>thesaurus onderwijsstructuur</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -955,7 +1045,7 @@
         <v>onderwijsstructuur</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -967,7 +1057,7 @@
         <v>onderwijsniveaus</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -979,7 +1069,7 @@
         <v>onderwijs subniveaus</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -991,7 +1081,7 @@
         <v>opleidingsvormen</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1003,7 +1093,7 @@
         <v>onderwijsgraden</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1015,7 +1105,7 @@
         <v>onderwijs leerjaren</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1027,7 +1117,7 @@
         <v>onderwijsstromen</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1039,7 +1129,7 @@
         <v>onderwijsfinaliteiten</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1051,7 +1141,7 @@
         <v>onderwijsvormen</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1066,7 +1156,7 @@
         <v>basisonderwijs</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1174,7 @@
         <v>kleuteronderwijs</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1105,7 +1195,7 @@
         <v>kleuter 3 jaar of jonger</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1126,7 +1216,7 @@
         <v>kleuter 4 jaar</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1147,7 +1237,7 @@
         <v>kleuter 5 jaar</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1165,7 +1255,7 @@
         <v>lager onderwijs</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -1185,8 +1275,11 @@
         <f t="shared" si="1"/>
         <v>lager 1e graad</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1209,8 +1302,11 @@
         <f t="shared" si="1"/>
         <v>lager 1e leerjaar</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1233,8 +1329,11 @@
         <f t="shared" si="1"/>
         <v>lager 2e leerjaar</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1254,8 +1353,11 @@
         <f t="shared" si="1"/>
         <v>lager 2e graad</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
@@ -1278,8 +1380,11 @@
         <f t="shared" si="1"/>
         <v>lager 3e leerjaar</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -1302,8 +1407,11 @@
         <f t="shared" si="1"/>
         <v>lager 4e leerjaar</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1323,8 +1431,11 @@
         <f t="shared" si="1"/>
         <v>lager 3e graad</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1347,8 +1458,11 @@
         <f t="shared" si="1"/>
         <v>lager 5e leerjaar</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1371,8 +1485,11 @@
         <f t="shared" si="1"/>
         <v>lager 6e leerjaar</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1504,7 @@
         <v>secundair onderwijs</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -1404,8 +1521,11 @@
         <f t="shared" si="1"/>
         <v>secundair 1e graad</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -1425,8 +1545,11 @@
         <f t="shared" si="1"/>
         <v>secundair 1e leerjaar</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -1446,8 +1569,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e leerjaar</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1467,8 +1593,11 @@
         <f t="shared" si="1"/>
         <v>secundair 1e graad a-stroom</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -1488,8 +1617,11 @@
         <f t="shared" si="1"/>
         <v>secundair 1e graad b-stroom</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1506,8 +1638,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>45</v>
       </c>
@@ -1527,8 +1662,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e leerjaar</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1548,8 +1686,11 @@
         <f t="shared" si="1"/>
         <v>secundair 4e leerjaar</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1569,8 +1710,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad finaliteit doorstroom</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1593,8 +1737,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad finaliteit doorstroom aso</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -1617,8 +1764,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad finaliteit doorstroom tso</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
@@ -1641,8 +1791,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad finaliteit doorstroom kso</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -1662,8 +1815,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad dubbele finaliteit</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -1686,8 +1842,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad dubbele finaliteit tso</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -1710,8 +1869,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad dubbele finaliteit kso</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -1731,8 +1893,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad finaliteit arbeidsmarkt</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1755,8 +1920,11 @@
         <f t="shared" si="1"/>
         <v>secundair 2e graad finaliteit arbeidsmarkt bso</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
@@ -1773,8 +1941,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1794,8 +1965,11 @@
         <f t="shared" si="1"/>
         <v>secundair 5e leerjaar</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1815,8 +1989,11 @@
         <f t="shared" si="1"/>
         <v>secundair 6e leerjaar</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -1836,8 +2013,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad finaliteit doorstroom</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
@@ -1860,8 +2040,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad finaliteit doorstroom aso</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>8</v>
       </c>
@@ -1884,8 +2067,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad finaliteit doorstroom tso</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
@@ -1908,8 +2094,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad finaliteit doorstroom kso</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -1929,8 +2118,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad dubbele finaliteit</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>8</v>
       </c>
@@ -1953,8 +2145,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad dubbele finaliteit tso</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
@@ -1977,8 +2172,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad dubbele finaliteit kso</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -1998,8 +2196,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad finaliteit arbeidsmarkt</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>8</v>
       </c>
@@ -2022,8 +2223,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad finaliteit arbeidsmarkt bso</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
@@ -2040,8 +2244,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad 3e leerjaar</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
@@ -2061,8 +2268,11 @@
         <f t="shared" si="1"/>
         <v>secundair 7e leerjaar</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -2082,8 +2292,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad 3e leerjaar finaliteit arbeidsmarkt</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>8</v>
       </c>
@@ -2106,8 +2319,11 @@
         <f t="shared" si="1"/>
         <v>secundair 3e graad 3e leerjaar finaliteit arbeidsmarkt bso</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L60" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>1</v>
       </c>
@@ -2121,8 +2337,9 @@
         <f t="shared" si="1"/>
         <v>buitengewoon basisonderwijs</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
@@ -2140,7 +2357,7 @@
         <v>buitengewoon kleuteronderwijs</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -2158,7 +2375,7 @@
         <v>buitengewoon lager onderwijs</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>1</v>
       </c>
@@ -2173,7 +2390,7 @@
         <v>buitengewoon secundair onderwijs</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>3</v>
       </c>
@@ -2184,14 +2401,17 @@
         <v>137</v>
       </c>
       <c r="J65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="K65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>buitengewoon secundair opleidingsvorm 1</v>
+      </c>
+      <c r="L65" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K65" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>opleidingsvorm 1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
@@ -2202,14 +2422,17 @@
         <v>139</v>
       </c>
       <c r="J66" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K66" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>buitengewoon secundair opleidingsvorm 2</v>
+      </c>
+      <c r="L66" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K66" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>opleidingsvorm 2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
@@ -2220,14 +2443,17 @@
         <v>141</v>
       </c>
       <c r="J67" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K67" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>buitengewoon secundair opleidingsvorm 3</v>
+      </c>
+      <c r="L67" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="K67" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>opleidingsvorm 3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -2238,14 +2464,17 @@
         <v>143</v>
       </c>
       <c r="J68" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K68" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>buitengewoon secundair opleidingsvorm 4</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="K68" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>opleidingsvorm 4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
@@ -2265,8 +2494,11 @@
         <f t="shared" si="1"/>
         <v>buitengewoon secundair 1e graad</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>145</v>
       </c>
@@ -2286,8 +2518,11 @@
         <f t="shared" si="1"/>
         <v>buitengewoon secundair 2e graad</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>145</v>
       </c>
@@ -2307,8 +2542,11 @@
         <f t="shared" si="1"/>
         <v>buitengewoon secundair 3e graad</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>145</v>
       </c>
@@ -2328,8 +2566,11 @@
         <f t="shared" si="1"/>
         <v>buitengewoon secundair 3e graad 3e leerjaar</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>1</v>
       </c>
@@ -2344,7 +2585,7 @@
         <v>volwassenenonderwijs</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>2</v>
       </c>
@@ -2362,7 +2603,7 @@
         <v>basiseducatie</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2621,7 @@
         <v>secundair volwassenenonderwijs</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>1</v>
       </c>
@@ -2395,7 +2636,7 @@
         <v>deeltijds kunstonderwijs</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>1</v>
       </c>
@@ -2412,7 +2653,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>